<commit_message>
Fix url jdv 264 (#224) faf4f41820064906ccb4e6566101ab6b8ba7e4e1
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-sdo-task.xlsx
+++ b/main/ig/StructureDefinition-sdo-task.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-27T09:57:43+00:00</t>
+    <t>2024-09-27T16:26:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1856,7 +1856,7 @@
     <t>Task.input:modePriseCharge.value[x]</t>
   </si>
   <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_J264-ModeEtCentreDePriseEnCharge-MDPH/FHIR/JDV_J264-ModeEtCentreDePriseEnCharge-MDPH</t>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J264-ModeEtCentreDePriseEnCharge-MDPH/FHIR/JDV-J264-ModeEtCentreDePriseEnCharge-MDPH</t>
   </si>
   <si>
     <t>Task.input:modePriseCharge.value[x].id</t>
@@ -2511,7 +2511,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="169.1328125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="123.9296875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="123.671875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
ANS-006-140 - RC Task - suppression du typedroitprestation (#287)
* Supression slice Task.typeDroitPrestation

* Suppression ligne droitPrestation dans la correspondance entre objets métiers et fhir

Suppression ligne droitPrestation dans la correspondance entre objets métiers et fhir 4d3fd204b620dce0a219eae08f0d4f6d800fe307
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-sdo-task.xlsx
+++ b/main/ig/StructureDefinition-sdo-task.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6219" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6003" uniqueCount="664">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-12T16:11:50+00:00</t>
+    <t>2024-12-12T16:13:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1417,7 +1417,7 @@
 </t>
   </si>
   <si>
-    <t>5</t>
+    <t>4</t>
   </si>
   <si>
     <t>Information used to perform task</t>
@@ -2031,41 +2031,6 @@
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J250-MotifStatutPersonnePriseChargeUnite/FHIR/JDV-J250-MotifStatutPersonnePriseChargeUnite</t>
-  </si>
-  <si>
-    <t>Task.input:typeDroitPrestation</t>
-  </si>
-  <si>
-    <t>typeDroitPrestation</t>
-  </si>
-  <si>
-    <t>Permet de définir le type de droit et prestation caractérisant la décision d'orientation.</t>
-  </si>
-  <si>
-    <t>Task.input:typeDroitPrestation.id</t>
-  </si>
-  <si>
-    <t>Task.input:typeDroitPrestation.extension</t>
-  </si>
-  <si>
-    <t>Task.input:typeDroitPrestation.modifierExtension</t>
-  </si>
-  <si>
-    <t>Task.input:typeDroitPrestation.type</t>
-  </si>
-  <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="https://interop.esante.gouv.fr/ig/fhir/sdo/CodeSystem/input-task-sdo-codesystem"/&gt;
-    &lt;code value="typeDroitPrestation"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>Task.input:typeDroitPrestation.value[x]</t>
-  </si>
-  <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_JXX-typeDroitPrestation/FHIR/JDV_JXX-typeDroitPrestation</t>
   </si>
   <si>
     <t>Task.input:idDecision</t>
@@ -2480,7 +2445,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN171"/>
+  <dimension ref="A1:AN165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -19938,7 +19903,7 @@
         <v>76</v>
       </c>
       <c r="K153" t="s" s="2">
-        <v>252</v>
+        <v>198</v>
       </c>
       <c r="L153" t="s" s="2">
         <v>468</v>
@@ -19971,11 +19936,13 @@
         <v>76</v>
       </c>
       <c r="X153" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="Y153" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="Y153" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="Z153" t="s" s="2">
-        <v>639</v>
+        <v>76</v>
       </c>
       <c r="AA153" t="s" s="2">
         <v>76</v>
@@ -20022,13 +19989,13 @@
     </row>
     <row r="154">
       <c r="A154" t="s" s="2">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B154" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C154" t="s" s="2">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D154" t="s" s="2">
         <v>449</v>
@@ -20053,7 +20020,7 @@
         <v>418</v>
       </c>
       <c r="L154" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="M154" t="s" s="2">
         <v>452</v>
@@ -20138,7 +20105,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s" s="2">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B155" t="s" s="2">
         <v>456</v>
@@ -20250,7 +20217,7 @@
     </row>
     <row r="156">
       <c r="A156" t="s" s="2">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B156" t="s" s="2">
         <v>457</v>
@@ -20364,7 +20331,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s" s="2">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B157" t="s" s="2">
         <v>458</v>
@@ -20480,7 +20447,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="2">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B158" t="s" s="2">
         <v>459</v>
@@ -20528,7 +20495,7 @@
         <v>76</v>
       </c>
       <c r="S158" t="s" s="2">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="T158" t="s" s="2">
         <v>76</v>
@@ -20596,7 +20563,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="2">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B159" t="s" s="2">
         <v>466</v>
@@ -20708,23 +20675,21 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="2">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B160" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="C160" t="s" s="2">
-        <v>650</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="C160" s="2"/>
       <c r="D160" t="s" s="2">
-        <v>449</v>
+        <v>76</v>
       </c>
       <c r="E160" s="2"/>
       <c r="F160" t="s" s="2">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G160" t="s" s="2">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H160" t="s" s="2">
         <v>76</v>
@@ -20739,14 +20704,14 @@
         <v>418</v>
       </c>
       <c r="L160" t="s" s="2">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="M160" t="s" s="2">
-        <v>452</v>
+        <v>650</v>
       </c>
       <c r="N160" s="2"/>
       <c r="O160" t="s" s="2">
-        <v>453</v>
+        <v>651</v>
       </c>
       <c r="P160" t="s" s="2">
         <v>76</v>
@@ -20795,7 +20760,7 @@
         <v>76</v>
       </c>
       <c r="AF160" t="s" s="2">
-        <v>448</v>
+        <v>648</v>
       </c>
       <c r="AG160" t="s" s="2">
         <v>77</v>
@@ -20827,7 +20792,7 @@
         <v>652</v>
       </c>
       <c r="B161" t="s" s="2">
-        <v>456</v>
+        <v>652</v>
       </c>
       <c r="C161" s="2"/>
       <c r="D161" t="s" s="2">
@@ -20939,7 +20904,7 @@
         <v>653</v>
       </c>
       <c r="B162" t="s" s="2">
-        <v>457</v>
+        <v>653</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" t="s" s="2">
@@ -21053,7 +21018,7 @@
         <v>654</v>
       </c>
       <c r="B163" t="s" s="2">
-        <v>458</v>
+        <v>654</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" t="s" s="2">
@@ -21169,7 +21134,7 @@
         <v>655</v>
       </c>
       <c r="B164" t="s" s="2">
-        <v>459</v>
+        <v>655</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" t="s" s="2">
@@ -21195,16 +21160,16 @@
         <v>252</v>
       </c>
       <c r="L164" t="s" s="2">
-        <v>461</v>
+        <v>656</v>
       </c>
       <c r="M164" t="s" s="2">
-        <v>462</v>
+        <v>657</v>
       </c>
       <c r="N164" t="s" s="2">
-        <v>463</v>
+        <v>262</v>
       </c>
       <c r="O164" t="s" s="2">
-        <v>464</v>
+        <v>658</v>
       </c>
       <c r="P164" t="s" s="2">
         <v>76</v>
@@ -21214,7 +21179,7 @@
         <v>76</v>
       </c>
       <c r="S164" t="s" s="2">
-        <v>656</v>
+        <v>76</v>
       </c>
       <c r="T164" t="s" s="2">
         <v>76</v>
@@ -21232,7 +21197,7 @@
         <v>156</v>
       </c>
       <c r="Y164" t="s" s="2">
-        <v>465</v>
+        <v>659</v>
       </c>
       <c r="Z164" t="s" s="2">
         <v>76</v>
@@ -21253,7 +21218,7 @@
         <v>76</v>
       </c>
       <c r="AF164" t="s" s="2">
-        <v>459</v>
+        <v>655</v>
       </c>
       <c r="AG164" t="s" s="2">
         <v>86</v>
@@ -21282,10 +21247,10 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="B165" t="s" s="2">
-        <v>466</v>
+        <v>660</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" t="s" s="2">
@@ -21308,16 +21273,18 @@
         <v>76</v>
       </c>
       <c r="K165" t="s" s="2">
-        <v>198</v>
+        <v>467</v>
       </c>
       <c r="L165" t="s" s="2">
-        <v>468</v>
+        <v>661</v>
       </c>
       <c r="M165" t="s" s="2">
-        <v>469</v>
+        <v>662</v>
       </c>
       <c r="N165" s="2"/>
-      <c r="O165" s="2"/>
+      <c r="O165" t="s" s="2">
+        <v>663</v>
+      </c>
       <c r="P165" t="s" s="2">
         <v>76</v>
       </c>
@@ -21365,7 +21332,7 @@
         <v>76</v>
       </c>
       <c r="AF165" t="s" s="2">
-        <v>466</v>
+        <v>660</v>
       </c>
       <c r="AG165" t="s" s="2">
         <v>86</v>
@@ -21389,692 +21356,6 @@
         <v>76</v>
       </c>
       <c r="AN165" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="s" s="2">
-        <v>658</v>
-      </c>
-      <c r="B166" t="s" s="2">
-        <v>658</v>
-      </c>
-      <c r="C166" s="2"/>
-      <c r="D166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E166" s="2"/>
-      <c r="F166" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G166" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K166" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="L166" t="s" s="2">
-        <v>659</v>
-      </c>
-      <c r="M166" t="s" s="2">
-        <v>660</v>
-      </c>
-      <c r="N166" s="2"/>
-      <c r="O166" t="s" s="2">
-        <v>661</v>
-      </c>
-      <c r="P166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q166" s="2"/>
-      <c r="R166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF166" t="s" s="2">
-        <v>658</v>
-      </c>
-      <c r="AG166" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH166" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI166" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ166" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL166" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="AM166" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN166" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="s" s="2">
-        <v>662</v>
-      </c>
-      <c r="B167" t="s" s="2">
-        <v>662</v>
-      </c>
-      <c r="C167" s="2"/>
-      <c r="D167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E167" s="2"/>
-      <c r="F167" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G167" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="H167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K167" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="L167" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="M167" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N167" s="2"/>
-      <c r="O167" s="2"/>
-      <c r="P167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q167" s="2"/>
-      <c r="R167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF167" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="AG167" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH167" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AI167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL167" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AM167" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN167" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="s" s="2">
-        <v>663</v>
-      </c>
-      <c r="B168" t="s" s="2">
-        <v>663</v>
-      </c>
-      <c r="C168" s="2"/>
-      <c r="D168" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="E168" s="2"/>
-      <c r="F168" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G168" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K168" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="L168" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="M168" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="N168" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="O168" s="2"/>
-      <c r="P168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q168" s="2"/>
-      <c r="R168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB168" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="AC168" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="AD168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE168" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="AF168" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="AG168" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH168" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI168" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ168" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="AK168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL168" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AM168" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN168" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="s" s="2">
-        <v>664</v>
-      </c>
-      <c r="B169" t="s" s="2">
-        <v>664</v>
-      </c>
-      <c r="C169" s="2"/>
-      <c r="D169" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="E169" s="2"/>
-      <c r="F169" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G169" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I169" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="J169" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="K169" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="L169" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="M169" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="N169" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="O169" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="P169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q169" s="2"/>
-      <c r="R169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF169" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="AG169" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH169" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI169" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ169" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="AK169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL169" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AM169" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN169" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="s" s="2">
-        <v>665</v>
-      </c>
-      <c r="B170" t="s" s="2">
-        <v>665</v>
-      </c>
-      <c r="C170" s="2"/>
-      <c r="D170" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="E170" s="2"/>
-      <c r="F170" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="G170" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="H170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K170" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="L170" t="s" s="2">
-        <v>666</v>
-      </c>
-      <c r="M170" t="s" s="2">
-        <v>667</v>
-      </c>
-      <c r="N170" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="O170" t="s" s="2">
-        <v>668</v>
-      </c>
-      <c r="P170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q170" s="2"/>
-      <c r="R170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X170" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y170" t="s" s="2">
-        <v>669</v>
-      </c>
-      <c r="Z170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF170" t="s" s="2">
-        <v>665</v>
-      </c>
-      <c r="AG170" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AH170" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AI170" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ170" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL170" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="AM170" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN170" t="s" s="2">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="s" s="2">
-        <v>670</v>
-      </c>
-      <c r="B171" t="s" s="2">
-        <v>670</v>
-      </c>
-      <c r="C171" s="2"/>
-      <c r="D171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E171" s="2"/>
-      <c r="F171" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="G171" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="H171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K171" t="s" s="2">
-        <v>467</v>
-      </c>
-      <c r="L171" t="s" s="2">
-        <v>671</v>
-      </c>
-      <c r="M171" t="s" s="2">
-        <v>672</v>
-      </c>
-      <c r="N171" s="2"/>
-      <c r="O171" t="s" s="2">
-        <v>673</v>
-      </c>
-      <c r="P171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q171" s="2"/>
-      <c r="R171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF171" t="s" s="2">
-        <v>670</v>
-      </c>
-      <c r="AG171" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AH171" t="s" s="2">
-        <v>86</v>
-      </c>
-      <c r="AI171" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="AJ171" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL171" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="AM171" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN171" t="s" s="2">
         <v>76</v>
       </c>
     </row>

</xml_diff>